<commit_message>
Updating website for Fall 2022
</commit_message>
<xml_diff>
--- a/data_extraction/Data Science Resources 20220816.xlsx
+++ b/data_extraction/Data Science Resources 20220816.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyle/Dropbox/Code/kylebradbury/data_extraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C04562-A98D-8E4B-876A-64CC9DC35614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF352D6-61E7-5C46-B062-3876EA6FD441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="500" windowWidth="13720" windowHeight="17500" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="500" windowWidth="26400" windowHeight="17500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2420" uniqueCount="1269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2426" uniqueCount="1274">
   <si>
     <t>Author</t>
   </si>
@@ -3852,6 +3852,21 @@
   </si>
   <si>
     <t>Awesome Machine Learning Research</t>
+  </si>
+  <si>
+    <t>https://eugeneyan.com/writing/design-patterns/?utm_source=substack&amp;utm_medium=email</t>
+  </si>
+  <si>
+    <t>Design Patterns in Machine Learning Code and Systems</t>
+  </si>
+  <si>
+    <t>https://ed-hawkins.github.io/climate-visuals/</t>
+  </si>
+  <si>
+    <t>https://github.com/sacridini/Awesome-Geospatial#python</t>
+  </si>
+  <si>
+    <t>Awesome Geospatial</t>
   </si>
 </sst>
 </file>
@@ -4235,9 +4250,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F73" sqref="F73"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6867,10 +6882,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3986E8D0-A3A6-904F-B22F-C7FF01277755}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6878,6 +6893,16 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1272</v>
       </c>
     </row>
   </sheetData>
@@ -6910,8 +6935,8 @@
   <dimension ref="A1:O69"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9348,9 +9373,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9777,7 +9802,7 @@
         <v>1024</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>9</v>
@@ -11201,11 +11226,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A104" sqref="A104"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12485,6 +12510,22 @@
       </c>
       <c r="B103" t="s">
         <v>1267</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>